<commit_message>
Baseline is modified, outputs included.
</commit_message>
<xml_diff>
--- a/output/Linear Regression/LR_results_python.xlsx
+++ b/output/Linear Regression/LR_results_python.xlsx
@@ -447,22 +447,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>5.670741422506266E+35</v>
+        <v>5.42754867889704E+35</v>
       </c>
       <c r="C2">
-        <v>1.587041102002215E+34</v>
+        <v>1.507261706098355E+34</v>
       </c>
       <c r="D2">
-        <v>2.026242939792716E+37</v>
+        <v>1.954424008956725E+37</v>
       </c>
       <c r="E2">
-        <v>77.7206279403413</v>
+        <v>77.67679566046903</v>
       </c>
       <c r="F2">
-        <v>1.824506951092196</v>
+        <v>1.828458224374995</v>
       </c>
       <c r="G2">
-        <v>42.59815392526501</v>
+        <v>42.4821276335261</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -473,25 +473,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>68.66348269975933</v>
+        <v>68.66095035333535</v>
       </c>
       <c r="C3">
-        <v>64.27934149131072</v>
+        <v>64.27688385548889</v>
       </c>
       <c r="D3">
-        <v>73.16462397626964</v>
+        <v>73.16201468195662</v>
       </c>
       <c r="E3">
-        <v>0.5227353171789323</v>
+        <v>0.5227203028711864</v>
       </c>
       <c r="F3">
-        <v>0.01343735843871683</v>
+        <v>0.01343733084017988</v>
       </c>
       <c r="G3">
-        <v>38.9016427270991</v>
+        <v>38.90060526813589</v>
       </c>
       <c r="H3">
-        <v>2.162104617517645E-306</v>
+        <v>2.238293274943599E-306</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -499,25 +499,25 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>110.5674029517208</v>
+        <v>110.5638495180865</v>
       </c>
       <c r="C4">
-        <v>94.58580498054994</v>
+        <v>94.5825747049449</v>
       </c>
       <c r="D4">
-        <v>127.8615913954478</v>
+        <v>127.8576835110027</v>
       </c>
       <c r="E4">
-        <v>0.7446356199261497</v>
+        <v>0.7446187442674873</v>
       </c>
       <c r="F4">
-        <v>0.04027172623694583</v>
+        <v>0.04027158606163192</v>
       </c>
       <c r="G4">
-        <v>18.49028312183476</v>
+        <v>18.4899284355952</v>
       </c>
       <c r="H4">
-        <v>5.760599788765747E-75</v>
+        <v>5.797234086427238E-75</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -525,25 +525,25 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>3.982818100576191</v>
+        <v>4.067043413890148</v>
       </c>
       <c r="C5">
-        <v>-1.318424243119487</v>
+        <v>-1.256454623025671</v>
       </c>
       <c r="D5">
-        <v>9.568846841033785</v>
+        <v>9.67754381881749</v>
       </c>
       <c r="E5">
-        <v>0.03905548893312868</v>
+        <v>0.03986515366736176</v>
       </c>
       <c r="F5">
-        <v>0.02669766073291734</v>
+        <v>0.02679045983757124</v>
       </c>
       <c r="G5">
-        <v>1.462880561852917</v>
+        <v>1.488035439072771</v>
       </c>
       <c r="H5">
-        <v>0.1435345654815635</v>
+        <v>0.1367761636417744</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -551,25 +551,25 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>387608.4852545148</v>
+        <v>387637.6638618933</v>
       </c>
       <c r="C6">
-        <v>189840.9772285312</v>
+        <v>189855.9516252367</v>
       </c>
       <c r="D6">
-        <v>791292.5248341353</v>
+        <v>791349.25279143</v>
       </c>
       <c r="E6">
-        <v>8.262838823566367</v>
+        <v>8.262914079875076</v>
       </c>
       <c r="F6">
-        <v>0.3640512004275385</v>
+        <v>0.3640493750762665</v>
       </c>
       <c r="G6">
-        <v>22.69691409851846</v>
+        <v>22.69723462138628</v>
       </c>
       <c r="H6">
-        <v>5.526182423507671E-111</v>
+        <v>5.488189412898144E-111</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -577,25 +577,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>-33.00760584664949</v>
+        <v>-32.97596724625498</v>
       </c>
       <c r="C7">
-        <v>-73.72549449958387</v>
+        <v>-73.71301499039156</v>
       </c>
       <c r="D7">
-        <v>70.81124036099531</v>
+        <v>70.89144932114073</v>
       </c>
       <c r="E7">
-        <v>-0.4005910931402656</v>
+        <v>-0.4001189330967176</v>
       </c>
       <c r="F7">
-        <v>0.4775408144986432</v>
+        <v>0.4775394401782307</v>
       </c>
       <c r="G7">
-        <v>-0.8388625243704773</v>
+        <v>-0.8378762033715631</v>
       </c>
       <c r="H7">
-        <v>0.4015684725083303</v>
+        <v>0.4021222186931896</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -603,25 +603,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>352.6519600974778</v>
+        <v>353.0136531720787</v>
       </c>
       <c r="C8">
-        <v>84.87867676853429</v>
+        <v>85.02603011760151</v>
       </c>
       <c r="D8">
-        <v>1008.260836573452</v>
+        <v>1009.14864157154</v>
       </c>
       <c r="E8">
-        <v>1.509953344195667</v>
+        <v>1.510752078493471</v>
       </c>
       <c r="F8">
-        <v>0.4568488374940309</v>
+        <v>0.4568498703891006</v>
       </c>
       <c r="G8">
-        <v>3.305148706250994</v>
+        <v>3.306889585427173</v>
       </c>
       <c r="H8">
-        <v>0.0009529280117179231</v>
+        <v>0.0009470329022164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>